<commit_message>
url encode permissions api parameters
</commit_message>
<xml_diff>
--- a/tests/integration/files/datasets/mcmd_person.xlsx
+++ b/tests/integration/files/datasets/mcmd_person.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommy/git/molgenis-tools-commander/tests/integration/files/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AA0DD4-D266-C140-892E-971118AFAAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC0035A-A75E-9547-ABB7-1F28C9AE713F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="3240" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="3240" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>firstName</t>
   </si>
@@ -99,17 +99,32 @@
     <t>person</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>mcmd_person</t>
+  </si>
+  <si>
+    <t>person/1</t>
+  </si>
+  <si>
+    <t>Bofke</t>
+  </si>
+  <si>
+    <t>Henkie</t>
+  </si>
+  <si>
+    <t>person?2</t>
+  </si>
+  <si>
+    <t>Piet</t>
+  </si>
+  <si>
+    <t>モルゲニス</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +157,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -644,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,10 +705,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -704,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -718,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -740,10 +761,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -806,7 +827,41 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>